<commit_message>
made draft functions in notebook to format outputs to JSON template
</commit_message>
<xml_diff>
--- a/testing/json_output/ConvertToJSONPlanning.xlsx
+++ b/testing/json_output/ConvertToJSONPlanning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dconly\GitRepos\PPA3\testing\json_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD63F4A-3441-4FDC-8D36-0674409ADBAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4AAB8F2-86EF-43B4-B309-B99B04735075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="705" windowWidth="24630" windowHeight="12915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="152">
   <si>
     <t>Report</t>
   </si>
@@ -492,6 +492,9 @@
   </si>
   <si>
     <t>lookup from region avgs table</t>
+  </si>
+  <si>
+    <t>landuse_buff_calcs.py</t>
   </si>
 </sst>
 </file>
@@ -849,7 +852,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,6 +911,9 @@
       <c r="D3" s="8" t="s">
         <v>116</v>
       </c>
+      <c r="E3" s="8" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -922,6 +928,9 @@
       <c r="D4" s="8" t="s">
         <v>115</v>
       </c>
+      <c r="E4" s="8" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -950,6 +959,9 @@
       <c r="D6" s="8" t="s">
         <v>116</v>
       </c>
+      <c r="E6" s="8" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
@@ -963,6 +975,9 @@
       </c>
       <c r="D7" s="8" t="s">
         <v>115</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">

</xml_diff>